<commit_message>
Avance Gestión de producción
Se crean archivos Markdown (readme y gestión de producción)
Se entregan VSM casi terminados
</commit_message>
<xml_diff>
--- a/Gestion Produccion/Tabla materiales y procesos.xlsx
+++ b/Gestion Produccion/Tabla materiales y procesos.xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="555" windowWidth="23100" windowHeight="9150"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Materiales" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Procesos" sheetId="2" r:id="rId5"/>
+    <sheet name="Materiales" sheetId="1" r:id="rId1"/>
+    <sheet name="Procesos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -29,12 +32,6 @@
     <t>Laca</t>
   </si>
   <si>
-    <t>Pegamento (poliuretano)</t>
-  </si>
-  <si>
-    <t>Tornillo #7 x 1 1/2"</t>
-  </si>
-  <si>
     <t>Tarugo madera 6x30 mm</t>
   </si>
   <si>
@@ -75,21 +72,28 @@
   </si>
   <si>
     <t>Paletizado</t>
+  </si>
+  <si>
+    <t>Pegamento (PVAc)</t>
+  </si>
+  <si>
+    <t>Tornillo #7 x 3/4"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -100,7 +104,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -116,7 +120,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -130,46 +140,39 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -359,31 +362,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.88"/>
-    <col customWidth="1" min="2" max="2" width="14.0"/>
-    <col customWidth="1" min="3" max="3" width="9.88"/>
-    <col customWidth="1" min="4" max="4" width="12.13"/>
-    <col customWidth="1" min="5" max="6" width="8.63"/>
-    <col customWidth="1" min="7" max="7" width="11.13"/>
-    <col customWidth="1" min="8" max="8" width="10.75"/>
-    <col customWidth="1" min="9" max="9" width="12.88"/>
-    <col customWidth="1" min="10" max="10" width="8.63"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,244 +408,245 @@
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.88"/>
-    <col customWidth="1" min="2" max="2" width="14.0"/>
-    <col customWidth="1" min="3" max="3" width="7.75"/>
-    <col customWidth="1" min="4" max="4" width="6.88"/>
-    <col customWidth="1" min="5" max="5" width="7.13"/>
-    <col customWidth="1" min="6" max="6" width="10.38"/>
-    <col customWidth="1" min="7" max="8" width="8.88"/>
-    <col customWidth="1" min="9" max="9" width="9.38"/>
-    <col customWidth="1" min="10" max="11" width="9.25"/>
-    <col customWidth="1" min="12" max="12" width="9.75"/>
-    <col customWidth="1" min="13" max="13" width="9.63"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>